<commit_message>
feat: implement tutorial text views
Also cleaned up a few bugs
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/tsv_UI_Tutorial.xlsx
+++ b/Assets/StreamingAssets/tsv_UI_Tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Unity Project\metho_misession_MarcSeb\Assets\StreamingAssets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FCCC713-D0E1-4BCB-A480-A367F31F33B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF5F75F0-C044-4794-98C9-11F8A079D354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Notes</t>
   </si>
@@ -152,6 +152,21 @@
   </si>
   <si>
     <t>A portal that spawns the level's boss.\nThe number at the bottom indicates the required currency to open it and call forth the boss.</t>
+  </si>
+  <si>
+    <t>tutorial</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Tutoriel</t>
+  </si>
+  <si>
+    <t>チュートリアル。</t>
+  </si>
+  <si>
+    <t>教程</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,27 +1085,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -1098,113 +1113,136 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>